<commit_message>
Day7, day8 and day9 updates.
</commit_message>
<xml_diff>
--- a/Day7/JOINS_loogika_kahe_tabeli_puhul.xlsx
+++ b/Day7/JOINS_loogika_kahe_tabeli_puhul.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcsk-my.sharepoint.com/personal/virve_rani_bcs_ee/Documents/Documents/Andmetarkus/Day7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{70788470-3D84-4242-B679-57C116F7D8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{434D9C05-17F9-4FAE-99ED-260484FB166F}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="8_{70788470-3D84-4242-B679-57C116F7D8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D26C8BB-1A57-4746-AD97-CDDF68BCE804}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-4020" windowWidth="19420" windowHeight="11500" xr2:uid="{C4777146-FCE6-4EDA-ADF6-ED4ABFDCD23F}"/>
+    <workbookView xWindow="-19310" yWindow="-4020" windowWidth="19420" windowHeight="11500" firstSheet="5" activeTab="7" xr2:uid="{C4777146-FCE6-4EDA-ADF6-ED4ABFDCD23F}"/>
   </bookViews>
   <sheets>
     <sheet name="Left join" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Left Join + Is null" sheetId="5" r:id="rId5"/>
     <sheet name="Right join + Is null" sheetId="6" r:id="rId6"/>
     <sheet name="Full outer join + is null" sheetId="8" r:id="rId7"/>
+    <sheet name="Mitu rida ühes tabelis" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="49">
   <si>
     <t>SalesRepTable</t>
   </si>
@@ -175,12 +176,54 @@
   <si>
     <t>Read, mis on puudu müügiesindaja tabelist või eelarve tabelist.</t>
   </si>
+  <si>
+    <t>LEFT JOIN</t>
+  </si>
+  <si>
+    <t>YearMonth</t>
+  </si>
+  <si>
+    <t>2025-01</t>
+  </si>
+  <si>
+    <t>2025-02</t>
+  </si>
+  <si>
+    <t>2025-03</t>
+  </si>
+  <si>
+    <t>SalesTable</t>
+  </si>
+  <si>
+    <t>SalesSum</t>
+  </si>
+  <si>
+    <t>SaleID</t>
+  </si>
+  <si>
+    <t>S001</t>
+  </si>
+  <si>
+    <t>S002</t>
+  </si>
+  <si>
+    <t>S003</t>
+  </si>
+  <si>
+    <t>S004</t>
+  </si>
+  <si>
+    <t>SELECT *
+ FROM BudgetTable 
+LEFT JOIN SalesTable
+ON BudgetTable.YearMonth = SalesTable.YearMonth</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,8 +240,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +285,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -248,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -262,6 +318,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C91FECC-ACAA-4EF0-9CBC-56BC4888A5AC}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1881,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875ADB16-7737-4FA4-919A-F5569141537D}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2048,4 +2107,246 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B24E220-A701-4481-9D50-2499BAF670C5}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.90625" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>4000</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>5000</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>4000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C9" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="D12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>4000</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>4000</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16">
+        <v>4000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>5000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>4000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>